<commit_message>
Add matlab results and poster
</commit_message>
<xml_diff>
--- a/Capstone/data/results/repDiffReport.xlsx
+++ b/Capstone/data/results/repDiffReport.xlsx
@@ -741,6 +741,15 @@
     <xf numFmtId="2" fontId="16" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -750,24 +759,15 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="16" fillId="33" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="33" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="A1:L12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,22 +1141,22 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="13"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="5">
         <v>0.5</v>
       </c>
@@ -1184,370 +1184,370 @@
       <c r="K2" s="6">
         <v>0.9</v>
       </c>
-      <c r="L2" s="16">
+      <c r="L2" s="13">
         <v>0.95</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>995</v>
+        <v>1678</v>
       </c>
       <c r="D3" s="2">
-        <v>995</v>
+        <v>1678</v>
       </c>
       <c r="E3" s="2">
-        <v>995</v>
+        <v>1678</v>
       </c>
       <c r="F3" s="2">
-        <v>997</v>
+        <v>1680</v>
       </c>
       <c r="G3" s="2">
-        <v>998</v>
+        <v>1681</v>
       </c>
       <c r="H3" s="2">
-        <v>1001</v>
+        <v>1684</v>
       </c>
       <c r="I3" s="2">
-        <v>1003</v>
+        <v>1686</v>
       </c>
       <c r="J3" s="2">
-        <v>1006</v>
+        <v>1689</v>
       </c>
       <c r="K3" s="2">
-        <v>1012</v>
-      </c>
-      <c r="L3" s="18">
-        <v>1024</v>
+        <v>1695</v>
+      </c>
+      <c r="L3" s="14">
+        <v>1707</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="19"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="8">
         <v>0.05</v>
       </c>
       <c r="C4" s="3">
-        <v>678</v>
+        <v>1125</v>
       </c>
       <c r="D4" s="4">
-        <v>678</v>
+        <v>1125</v>
       </c>
       <c r="E4" s="4">
-        <v>681</v>
+        <v>1128</v>
       </c>
       <c r="F4" s="4">
-        <v>685</v>
+        <v>1132</v>
       </c>
       <c r="G4" s="4">
-        <v>690</v>
+        <v>1137</v>
       </c>
       <c r="H4" s="4">
-        <v>703</v>
+        <v>1150</v>
       </c>
       <c r="I4" s="4">
-        <v>716</v>
+        <v>1163</v>
       </c>
       <c r="J4" s="4">
-        <v>735</v>
+        <v>1182</v>
       </c>
       <c r="K4" s="4">
-        <v>762</v>
-      </c>
-      <c r="L4" s="20">
-        <v>789</v>
+        <v>1209</v>
+      </c>
+      <c r="L4" s="15">
+        <v>1236</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="8">
         <v>0.1</v>
       </c>
       <c r="C5" s="3">
-        <v>496</v>
+        <v>541</v>
       </c>
       <c r="D5" s="4">
-        <v>499</v>
+        <v>540</v>
       </c>
       <c r="E5" s="4">
-        <v>503</v>
+        <v>542</v>
       </c>
       <c r="F5" s="4">
-        <v>513</v>
+        <v>552</v>
       </c>
       <c r="G5" s="4">
-        <v>521</v>
+        <v>560</v>
       </c>
       <c r="H5" s="4">
-        <v>553</v>
+        <v>586</v>
       </c>
       <c r="I5" s="4">
-        <v>579</v>
+        <v>608</v>
       </c>
       <c r="J5" s="4">
-        <v>611</v>
+        <v>638</v>
       </c>
       <c r="K5" s="4">
-        <v>650</v>
-      </c>
-      <c r="L5" s="20">
-        <v>686</v>
+        <v>707</v>
+      </c>
+      <c r="L5" s="15">
+        <v>785</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="8">
         <v>0.15</v>
       </c>
       <c r="C6" s="3">
-        <v>413</v>
+        <v>477</v>
       </c>
       <c r="D6" s="4">
-        <v>418</v>
+        <v>476</v>
       </c>
       <c r="E6" s="4">
-        <v>425</v>
+        <v>479</v>
       </c>
       <c r="F6" s="4">
-        <v>440</v>
+        <v>488</v>
       </c>
       <c r="G6" s="4">
-        <v>453</v>
+        <v>499</v>
       </c>
       <c r="H6" s="4">
-        <v>491</v>
+        <v>529</v>
       </c>
       <c r="I6" s="4">
-        <v>523</v>
+        <v>551</v>
       </c>
       <c r="J6" s="4">
-        <v>559</v>
+        <v>575</v>
       </c>
       <c r="K6" s="4">
-        <v>599</v>
-      </c>
-      <c r="L6" s="20">
-        <v>640</v>
+        <v>643</v>
+      </c>
+      <c r="L6" s="15">
+        <v>727</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="8">
         <v>0.2</v>
       </c>
       <c r="C7" s="3">
-        <v>372</v>
+        <v>462</v>
       </c>
       <c r="D7" s="4">
-        <v>383</v>
+        <v>463</v>
       </c>
       <c r="E7" s="4">
-        <v>393</v>
+        <v>467</v>
       </c>
       <c r="F7" s="4">
-        <v>409</v>
+        <v>477</v>
       </c>
       <c r="G7" s="4">
-        <v>424</v>
+        <v>488</v>
       </c>
       <c r="H7" s="4">
-        <v>463</v>
+        <v>515</v>
       </c>
       <c r="I7" s="4">
-        <v>495</v>
+        <v>537</v>
       </c>
       <c r="J7" s="4">
-        <v>531</v>
+        <v>561</v>
       </c>
       <c r="K7" s="4">
-        <v>573</v>
-      </c>
-      <c r="L7" s="20">
-        <v>615</v>
+        <v>631</v>
+      </c>
+      <c r="L7" s="15">
+        <v>708</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="8">
         <v>0.25</v>
       </c>
       <c r="C8" s="3">
-        <v>353</v>
+        <v>455</v>
       </c>
       <c r="D8" s="4">
-        <v>369</v>
+        <v>455</v>
       </c>
       <c r="E8" s="4">
-        <v>379</v>
+        <v>459</v>
       </c>
       <c r="F8" s="4">
-        <v>397</v>
+        <v>471</v>
       </c>
       <c r="G8" s="4">
-        <v>413</v>
+        <v>483</v>
       </c>
       <c r="H8" s="4">
-        <v>453</v>
+        <v>507</v>
       </c>
       <c r="I8" s="4">
-        <v>487</v>
+        <v>531</v>
       </c>
       <c r="J8" s="4">
-        <v>523</v>
+        <v>555</v>
       </c>
       <c r="K8" s="4">
-        <v>566</v>
-      </c>
-      <c r="L8" s="20">
-        <v>609</v>
+        <v>624</v>
+      </c>
+      <c r="L8" s="15">
+        <v>702</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="8">
         <v>0.3</v>
       </c>
       <c r="C9" s="3">
-        <v>306</v>
+        <v>462</v>
       </c>
       <c r="D9" s="4">
-        <v>336</v>
+        <v>456</v>
       </c>
       <c r="E9" s="4">
-        <v>356</v>
+        <v>458</v>
       </c>
       <c r="F9" s="4">
-        <v>375</v>
+        <v>469</v>
       </c>
       <c r="G9" s="4">
-        <v>399</v>
+        <v>477</v>
       </c>
       <c r="H9" s="4">
-        <v>441</v>
+        <v>501</v>
       </c>
       <c r="I9" s="4">
-        <v>478</v>
+        <v>524</v>
       </c>
       <c r="J9" s="4">
-        <v>514</v>
+        <v>548</v>
       </c>
       <c r="K9" s="4">
-        <v>557</v>
-      </c>
-      <c r="L9" s="20">
-        <v>601</v>
+        <v>617</v>
+      </c>
+      <c r="L9" s="15">
+        <v>696</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="8">
         <v>0.35</v>
       </c>
       <c r="C10" s="3">
-        <v>229</v>
+        <v>471</v>
       </c>
       <c r="D10" s="4">
-        <v>289</v>
+        <v>451</v>
       </c>
       <c r="E10" s="4">
-        <v>324</v>
+        <v>450</v>
       </c>
       <c r="F10" s="4">
-        <v>348</v>
+        <v>462</v>
       </c>
       <c r="G10" s="4">
-        <v>377</v>
+        <v>465</v>
       </c>
       <c r="H10" s="4">
-        <v>425</v>
+        <v>491</v>
       </c>
       <c r="I10" s="4">
-        <v>463</v>
+        <v>513</v>
       </c>
       <c r="J10" s="4">
-        <v>501</v>
+        <v>539</v>
       </c>
       <c r="K10" s="4">
-        <v>544</v>
-      </c>
-      <c r="L10" s="20">
-        <v>589</v>
+        <v>608</v>
+      </c>
+      <c r="L10" s="15">
+        <v>686</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="8">
         <v>0.4</v>
       </c>
       <c r="C11" s="3">
-        <v>91</v>
+        <v>539</v>
       </c>
       <c r="D11" s="4">
-        <v>213</v>
+        <v>463</v>
       </c>
       <c r="E11" s="4">
-        <v>273</v>
+        <v>459</v>
       </c>
       <c r="F11" s="4">
-        <v>312</v>
+        <v>462</v>
       </c>
       <c r="G11" s="4">
-        <v>350</v>
+        <v>466</v>
       </c>
       <c r="H11" s="4">
-        <v>404</v>
+        <v>486</v>
       </c>
       <c r="I11" s="4">
-        <v>442</v>
+        <v>508</v>
       </c>
       <c r="J11" s="4">
-        <v>480</v>
+        <v>534</v>
       </c>
       <c r="K11" s="4">
-        <v>526</v>
-      </c>
-      <c r="L11" s="20">
-        <v>571</v>
+        <v>602</v>
+      </c>
+      <c r="L11" s="15">
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22">
+      <c r="A12" s="25"/>
+      <c r="B12" s="16">
         <v>0.45</v>
       </c>
-      <c r="C12" s="23">
-        <v>-208</v>
-      </c>
-      <c r="D12" s="24">
-        <v>100</v>
-      </c>
-      <c r="E12" s="24">
-        <v>206</v>
-      </c>
-      <c r="F12" s="24">
-        <v>268</v>
-      </c>
-      <c r="G12" s="24">
-        <v>318</v>
-      </c>
-      <c r="H12" s="24">
-        <v>383</v>
-      </c>
-      <c r="I12" s="24">
-        <v>428</v>
-      </c>
-      <c r="J12" s="24">
-        <v>466</v>
-      </c>
-      <c r="K12" s="24">
-        <v>516</v>
-      </c>
-      <c r="L12" s="25">
-        <v>561</v>
+      <c r="C12" s="17">
+        <v>766</v>
+      </c>
+      <c r="D12" s="18">
+        <v>512</v>
+      </c>
+      <c r="E12" s="18">
+        <v>464</v>
+      </c>
+      <c r="F12" s="18">
+        <v>454</v>
+      </c>
+      <c r="G12" s="18">
+        <v>450</v>
+      </c>
+      <c r="H12" s="18">
+        <v>475</v>
+      </c>
+      <c r="I12" s="18">
+        <v>498</v>
+      </c>
+      <c r="J12" s="18">
+        <v>524</v>
+      </c>
+      <c r="K12" s="18">
+        <v>594</v>
+      </c>
+      <c r="L12" s="19">
+        <v>670</v>
       </c>
     </row>
   </sheetData>
@@ -1559,11 +1559,9 @@
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="num" val="0"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FF92D050"/>
-        <color rgb="FF7030A0"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFC00000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>